<commit_message>
update botly user data
</commit_message>
<xml_diff>
--- a/import/datastore/users.xlsx
+++ b/import/datastore/users.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="98">
   <si>
     <t>ski</t>
   </si>
@@ -310,6 +310,21 @@
   </si>
   <si>
     <t>U5LL0BN4U:T5C4WRWET</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>default-user</t>
+  </si>
+  <si>
+    <t>Botly</t>
+  </si>
+  <si>
+    <t>Emulator</t>
+  </si>
+  <si>
+    <t>Bot</t>
   </si>
 </sst>
 </file>
@@ -489,7 +504,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -501,6 +516,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -643,7 +659,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -698,7 +714,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -753,7 +769,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -810,7 +826,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -867,7 +883,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -924,7 +940,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -979,7 +995,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1036,7 +1052,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1091,7 +1107,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1148,7 +1164,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1205,7 +1221,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1262,7 +1278,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1317,7 +1333,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1374,7 +1390,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1429,7 +1445,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1484,7 +1500,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1539,7 +1555,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1596,7 +1612,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1651,7 +1667,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1706,7 +1722,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1763,7 +1779,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1818,7 +1834,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1873,7 +1889,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1930,7 +1946,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1987,7 +2003,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2044,7 +2060,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2099,7 +2115,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2156,7 +2172,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2211,7 +2227,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2266,7 +2282,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2321,7 +2337,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2378,7 +2394,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2433,7 +2449,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2488,7 +2504,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2545,7 +2561,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2600,7 +2616,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2655,7 +2671,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2712,7 +2728,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2769,7 +2785,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2826,7 +2842,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3165,7 +3181,7 @@
   <dimension ref="A1:AD47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3426,63 +3442,63 @@
         <v>{</v>
       </c>
       <c r="P5" t="str">
-        <f>IF(P$4=0,O5,O5&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A5&amp;"""",IF(P$3=2,IF(A5=1,"true", "false"),A5))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" ref="P5:P46" si="1">IF(P$4=0,O5,O5&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A5&amp;"""",IF(P$3=2,IF(A5=1,"true", "false"),A5))&amp;IF(ISBLANK(Q$3),"},",""))</f>
         <v>{"user":"meyerchri"</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" ref="Q5:AC5" si="1">IF(Q$4=0,P5,P5&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B5&amp;"""",IF(Q$3=2,IF(B5=1,"true", "false"),B5))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q5:AC5" si="2">IF(Q$4=0,P5,P5&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B5&amp;"""",IF(Q$3=2,IF(B5=1,"true", "false"),B5))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET"</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer"</v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina"</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13"</v>
       </c>
       <c r="U5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0"</v>
       </c>
       <c r="V5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation"</v>
       </c>
       <c r="W5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60"</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f"</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133"</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation"</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
       </c>
       <c r="AD5" t="str">
-        <f>IF(ISBLANK(C5),"",AC5&amp;"}"&amp;IF(OR(AD6="]",AD6="",ISBLANK(AD6)),"",","))</f>
+        <f t="shared" ref="AD5:AD12" si="3">IF(ISBLANK(C5),"",AC5&amp;"}"&amp;IF(OR(AD6="]",AD6="",ISBLANK(AD6)),"",","))</f>
         <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"},</v>
       </c>
     </row>
@@ -3524,67 +3540,67 @@
         <v>65</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" ref="O6:O46" si="2">"{"</f>
+        <f t="shared" ref="O6:O46" si="4">"{"</f>
         <v>{</v>
       </c>
       <c r="P6" t="str">
-        <f>IF(P$4=0,O6,O6&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A6&amp;"""",IF(P$3=2,IF(A6=1,"true", "false"),A6))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"david"</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" ref="Q6:AC6" si="3">IF(Q$4=0,P6,P6&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B6&amp;"""",IF(Q$3=2,IF(B6=1,"true", "false"),B6))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q6:AC6" si="5">IF(Q$4=0,P6,P6&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B6&amp;"""",IF(Q$3=2,IF(B6=1,"true", "false"),B6))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET"</v>
       </c>
       <c r="R6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich"</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David"</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01"</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50"</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture"</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90"</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m"</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327"</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit"</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+      </c>
+      <c r="AC6" t="str">
+        <f t="shared" si="5"/>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+      </c>
+      <c r="AD6" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich"</v>
-      </c>
-      <c r="S6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David"</v>
-      </c>
-      <c r="T6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01"</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50"</v>
-      </c>
-      <c r="V6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture"</v>
-      </c>
-      <c r="W6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90"</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m"</v>
-      </c>
-      <c r="Y6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327"</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit"</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
-      </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
-      </c>
-      <c r="AC6" t="str">
-        <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
-      </c>
-      <c r="AD6" t="str">
-        <f>IF(ISBLANK(C6),"",AC6&amp;"}"&amp;IF(OR(AD7="]",AD7="",ISBLANK(AD7)),"",","))</f>
         <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"},</v>
       </c>
     </row>
@@ -3626,67 +3642,67 @@
         <v>53</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P7" t="str">
-        <f>IF(P$4=0,O7,O7&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A7&amp;"""",IF(P$3=2,IF(A7=1,"true", "false"),A7))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"remostrupler"</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" ref="Q7:AC7" si="4">IF(Q$4=0,P7,P7&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B7&amp;"""",IF(Q$3=2,IF(B7=1,"true", "false"),B7))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q7:AC7" si="6">IF(Q$4=0,P7,P7&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B7&amp;"""",IF(Q$3=2,IF(B7=1,"true", "false"),B7))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET"</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler"</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo"</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01"</v>
       </c>
       <c r="U7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0"</v>
       </c>
       <c r="V7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk"</v>
       </c>
       <c r="W7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100"</v>
       </c>
       <c r="X7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328"</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man."</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
       </c>
       <c r="AC7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
       </c>
       <c r="AD7" t="str">
-        <f>IF(ISBLANK(C7),"",AC7&amp;"}"&amp;IF(OR(AD8="]",AD8="",ISBLANK(AD8)),"",","))</f>
+        <f t="shared" si="3"/>
         <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"},</v>
       </c>
     </row>
@@ -3728,67 +3744,67 @@
         <v>53</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P8" t="str">
-        <f>IF(P$4=0,O8,O8&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A8&amp;"""",IF(P$3=2,IF(A8=1,"true", "false"),A8))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"susanne_s"</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" ref="Q8:AC8" si="5">IF(Q$4=0,P8,P8&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B8&amp;"""",IF(Q$3=2,IF(B8=1,"true", "false"),B8))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q8:AC8" si="7">IF(Q$4=0,P8,P8&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B8&amp;"""",IF(Q$3=2,IF(B8=1,"true", "false"),B8))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET"</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer"</v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne"</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01"</v>
       </c>
       <c r="U8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0"</v>
       </c>
       <c r="V8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR"</v>
       </c>
       <c r="W8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100"</v>
       </c>
       <c r="X8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f"</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201"</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services"</v>
       </c>
       <c r="AA8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
       </c>
       <c r="AC8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
       </c>
       <c r="AD8" t="str">
-        <f>IF(ISBLANK(C8),"",AC8&amp;"}"&amp;IF(OR(AD9="]",AD9="",ISBLANK(AD9)),"",","))</f>
+        <f t="shared" si="3"/>
         <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"},</v>
       </c>
     </row>
@@ -3830,67 +3846,67 @@
         <v>53</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P9" t="str">
-        <f>IF(P$4=0,O9,O9&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A9&amp;"""",IF(P$3=2,IF(A9=1,"true", "false"),A9))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"lorenz-haenggi"</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" ref="Q9:AC9" si="6">IF(Q$4=0,P9,P9&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B9&amp;"""",IF(Q$3=2,IF(B9=1,"true", "false"),B9))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q9:AC9" si="8">IF(Q$4=0,P9,P9&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B9&amp;"""",IF(Q$3=2,IF(B9=1,"true", "false"),B9))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET"</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi"</v>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz"</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13"</v>
       </c>
       <c r="U9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50"</v>
       </c>
       <c r="V9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation"</v>
       </c>
       <c r="W9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100"</v>
       </c>
       <c r="X9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323"</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA"</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
       </c>
       <c r="AC9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
       </c>
       <c r="AD9" t="str">
-        <f>IF(ISBLANK(C9),"",AC9&amp;"}"&amp;IF(OR(AD10="]",AD10="",ISBLANK(AD10)),"",","))</f>
+        <f t="shared" si="3"/>
         <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"},</v>
       </c>
     </row>
@@ -3932,67 +3948,67 @@
         <v>53</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P10" t="str">
-        <f>IF(P$4=0,O10,O10&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A10&amp;"""",IF(P$3=2,IF(A10=1,"true", "false"),A10))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"cogji"</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" ref="Q10:AC10" si="7">IF(Q$4=0,P10,P10&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B10&amp;"""",IF(Q$3=2,IF(B10=1,"true", "false"),B10))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q10:AC10" si="9">IF(Q$4=0,P10,P10&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B10&amp;"""",IF(Q$3=2,IF(B10=1,"true", "false"),B10))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET"</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi"</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne"</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01"</v>
       </c>
       <c r="U10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0"</v>
       </c>
       <c r="V10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR"</v>
       </c>
       <c r="W10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80"</v>
       </c>
       <c r="X10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f"</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222"</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development"</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
       </c>
       <c r="AD10" t="str">
-        <f>IF(ISBLANK(C10),"",AC10&amp;"}"&amp;IF(OR(AD11="]",AD11="",ISBLANK(AD11)),"",","))</f>
+        <f t="shared" si="3"/>
         <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"},</v>
       </c>
     </row>
@@ -4034,195 +4050,231 @@
         <v>53</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P11" t="str">
-        <f>IF(P$4=0,O11,O11&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A11&amp;"""",IF(P$3=2,IF(A11=1,"true", "false"),A11))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":"brm"</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:AC11" si="8">IF(Q$4=0,P11,P11&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B11&amp;"""",IF(Q$3=2,IF(B11=1,"true", "false"),B11))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q11:AC11" si="10">IF(Q$4=0,P11,P11&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B11&amp;"""",IF(Q$3=2,IF(B11=1,"true", "false"),B11))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET"</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser"</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard"</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01"</v>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0"</v>
       </c>
       <c r="V11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist"</v>
       </c>
       <c r="W11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100"</v>
       </c>
       <c r="X11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001"</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services"</v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
       </c>
       <c r="AD11" t="str">
-        <f>IF(ISBLANK(C11),"",AC11&amp;"}"&amp;IF(OR(AD12="]",AD12="",ISBLANK(AD12)),"",","))</f>
-        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"}</v>
+        <f t="shared" si="3"/>
+        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"},</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="11">
+        <v>42894</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12">
+        <v>18222</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
       <c r="O12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P12" t="str">
-        <f>IF(P$4=0,O12,O12&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A12&amp;"""",IF(P$3=2,IF(A12=1,"true", "false"),A12))&amp;IF(ISBLANK(Q$3),"},",""))</f>
-        <v>{"user":""</v>
+        <f t="shared" si="1"/>
+        <v>{"user":"User"</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" ref="Q12:AC12" si="9">IF(Q$4=0,P12,P12&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B12&amp;"""",IF(Q$3=2,IF(B12=1,"true", "false"),B12))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"","slack_id":""</v>
+        <f t="shared" ref="Q12:AC12" si="11">IF(Q$4=0,P12,P12&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B12&amp;"""",IF(Q$3=2,IF(B12=1,"true", "false"),B12))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <v>{"user":"User","slack_id":"default-user"</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator"</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly"</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894"</v>
       </c>
       <c r="U12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0"</v>
       </c>
       <c r="V12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot"</v>
       </c>
       <c r="W12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100"</v>
       </c>
       <c r="X12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222"</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot"</v>
       </c>
       <c r="AA12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="9"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <f t="shared" si="11"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
       </c>
       <c r="AD12" t="str">
-        <f>IF(ISBLANK(C12),"",AC12&amp;"}"&amp;IF(OR(AD13="]",AD13="",ISBLANK(AD13)),"",","))</f>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"}</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="O13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P13" t="str">
-        <f>IF(P$4=0,O13,O13&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A13&amp;"""",IF(P$3=2,IF(A13=1,"true", "false"),A13))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" ref="Q13:AC13" si="10">IF(Q$4=0,P13,P13&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B13&amp;"""",IF(Q$3=2,IF(B13=1,"true", "false"),B13))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q13:AC13" si="12">IF(Q$4=0,P13,P13&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B13&amp;"""",IF(Q$3=2,IF(B13=1,"true", "false"),B13))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD13" t="str">
@@ -4232,2179 +4284,2179 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="O14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P14" t="str">
-        <f>IF(P$4=0,O14,O14&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A14&amp;"""",IF(P$3=2,IF(A14=1,"true", "false"),A14))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" ref="Q14:AC14" si="11">IF(Q$4=0,P14,P14&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B14&amp;"""",IF(Q$3=2,IF(B14=1,"true", "false"),B14))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q14:AC14" si="13">IF(Q$4=0,P14,P14&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B14&amp;"""",IF(Q$3=2,IF(B14=1,"true", "false"),B14))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD14" t="str">
-        <f>IF(ISBLANK(C14),"",AC14&amp;"}"&amp;IF(OR(AD15="]",AD15="",ISBLANK(AD15)),"",","))</f>
+        <f t="shared" ref="AD14:AD46" si="14">IF(ISBLANK(C14),"",AC14&amp;"}"&amp;IF(OR(AD15="]",AD15="",ISBLANK(AD15)),"",","))</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="O15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P15" t="str">
-        <f>IF(P$4=0,O15,O15&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A15&amp;"""",IF(P$3=2,IF(A15=1,"true", "false"),A15))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" ref="Q15:AC15" si="12">IF(Q$4=0,P15,P15&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B15&amp;"""",IF(Q$3=2,IF(B15=1,"true", "false"),B15))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q15:AC15" si="15">IF(Q$4=0,P15,P15&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B15&amp;"""",IF(Q$3=2,IF(B15=1,"true", "false"),B15))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD15" t="str">
-        <f>IF(ISBLANK(C15),"",AC15&amp;"}"&amp;IF(OR(AD16="]",AD16="",ISBLANK(AD16)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="O16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P16" t="str">
-        <f>IF(P$4=0,O16,O16&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A16&amp;"""",IF(P$3=2,IF(A16=1,"true", "false"),A16))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" ref="Q16:AC16" si="13">IF(Q$4=0,P16,P16&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B16&amp;"""",IF(Q$3=2,IF(B16=1,"true", "false"),B16))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q16:AC16" si="16">IF(Q$4=0,P16,P16&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B16&amp;"""",IF(Q$3=2,IF(B16=1,"true", "false"),B16))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC16" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD16" t="str">
-        <f>IF(ISBLANK(C16),"",AC16&amp;"}"&amp;IF(OR(AD17="]",AD17="",ISBLANK(AD17)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P17" t="str">
-        <f>IF(P$4=0,O17,O17&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A17&amp;"""",IF(P$3=2,IF(A17=1,"true", "false"),A17))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" ref="Q17:AC17" si="14">IF(Q$4=0,P17,P17&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B17&amp;"""",IF(Q$3=2,IF(B17=1,"true", "false"),B17))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q17:AC17" si="17">IF(Q$4=0,P17,P17&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B17&amp;"""",IF(Q$3=2,IF(B17=1,"true", "false"),B17))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":""</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":""</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
+      </c>
+      <c r="X17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
+      </c>
+      <c r="Z17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+      </c>
+      <c r="AC17" t="str">
+        <f t="shared" si="17"/>
+        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+      </c>
+      <c r="AD17" t="str">
         <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":""</v>
-      </c>
-      <c r="S17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":""</v>
-      </c>
-      <c r="T17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
-      </c>
-      <c r="U17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
-      </c>
-      <c r="V17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
-      </c>
-      <c r="W17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
-      </c>
-      <c r="X17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
-      </c>
-      <c r="Y17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
-      </c>
-      <c r="Z17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
-      </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
-      </c>
-      <c r="AB17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
-      </c>
-      <c r="AC17" t="str">
-        <f t="shared" si="14"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
-      </c>
-      <c r="AD17" t="str">
-        <f>IF(ISBLANK(C17),"",AC17&amp;"}"&amp;IF(OR(AD18="]",AD18="",ISBLANK(AD18)),"",","))</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P18" t="str">
-        <f>IF(P$4=0,O18,O18&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A18&amp;"""",IF(P$3=2,IF(A18=1,"true", "false"),A18))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" ref="Q18:AC18" si="15">IF(Q$4=0,P18,P18&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B18&amp;"""",IF(Q$3=2,IF(B18=1,"true", "false"),B18))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q18:AC18" si="18">IF(Q$4=0,P18,P18&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B18&amp;"""",IF(Q$3=2,IF(B18=1,"true", "false"),B18))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD18" t="str">
-        <f>IF(ISBLANK(C18),"",AC18&amp;"}"&amp;IF(OR(AD19="]",AD19="",ISBLANK(AD19)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P19" t="str">
-        <f>IF(P$4=0,O19,O19&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A19&amp;"""",IF(P$3=2,IF(A19=1,"true", "false"),A19))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" ref="Q19:AC19" si="16">IF(Q$4=0,P19,P19&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B19&amp;"""",IF(Q$3=2,IF(B19=1,"true", "false"),B19))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q19:AC19" si="19">IF(Q$4=0,P19,P19&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B19&amp;"""",IF(Q$3=2,IF(B19=1,"true", "false"),B19))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD19" t="str">
-        <f>IF(ISBLANK(C19),"",AC19&amp;"}"&amp;IF(OR(AD20="]",AD20="",ISBLANK(AD20)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P20" t="str">
-        <f>IF(P$4=0,O20,O20&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A20&amp;"""",IF(P$3=2,IF(A20=1,"true", "false"),A20))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ref="Q20:AC20" si="17">IF(Q$4=0,P20,P20&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B20&amp;"""",IF(Q$3=2,IF(B20=1,"true", "false"),B20))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q20:AC20" si="20">IF(Q$4=0,P20,P20&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B20&amp;"""",IF(Q$3=2,IF(B20=1,"true", "false"),B20))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD20" t="str">
-        <f>IF(ISBLANK(C20),"",AC20&amp;"}"&amp;IF(OR(AD21="]",AD21="",ISBLANK(AD21)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P21" t="str">
-        <f>IF(P$4=0,O21,O21&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A21&amp;"""",IF(P$3=2,IF(A21=1,"true", "false"),A21))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" ref="Q21:AC21" si="18">IF(Q$4=0,P21,P21&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B21&amp;"""",IF(Q$3=2,IF(B21=1,"true", "false"),B21))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q21:AC21" si="21">IF(Q$4=0,P21,P21&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B21&amp;"""",IF(Q$3=2,IF(B21=1,"true", "false"),B21))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC21" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD21" t="str">
-        <f>IF(ISBLANK(C21),"",AC21&amp;"}"&amp;IF(OR(AD22="]",AD22="",ISBLANK(AD22)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P22" t="str">
-        <f>IF(P$4=0,O22,O22&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A22&amp;"""",IF(P$3=2,IF(A22=1,"true", "false"),A22))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22:AC22" si="19">IF(Q$4=0,P22,P22&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B22&amp;"""",IF(Q$3=2,IF(B22=1,"true", "false"),B22))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q22:AC22" si="22">IF(Q$4=0,P22,P22&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B22&amp;"""",IF(Q$3=2,IF(B22=1,"true", "false"),B22))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC22" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD22" t="str">
-        <f>IF(ISBLANK(C22),"",AC22&amp;"}"&amp;IF(OR(AD23="]",AD23="",ISBLANK(AD23)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P23" t="str">
-        <f>IF(P$4=0,O23,O23&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A23&amp;"""",IF(P$3=2,IF(A23=1,"true", "false"),A23))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" ref="Q23:AC23" si="20">IF(Q$4=0,P23,P23&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B23&amp;"""",IF(Q$3=2,IF(B23=1,"true", "false"),B23))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q23:AC23" si="23">IF(Q$4=0,P23,P23&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B23&amp;"""",IF(Q$3=2,IF(B23=1,"true", "false"),B23))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC23" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD23" t="str">
-        <f>IF(ISBLANK(C23),"",AC23&amp;"}"&amp;IF(OR(AD24="]",AD24="",ISBLANK(AD24)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P24" t="str">
-        <f>IF(P$4=0,O24,O24&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A24&amp;"""",IF(P$3=2,IF(A24=1,"true", "false"),A24))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" ref="Q24:AC24" si="21">IF(Q$4=0,P24,P24&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B24&amp;"""",IF(Q$3=2,IF(B24=1,"true", "false"),B24))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q24:AC24" si="24">IF(Q$4=0,P24,P24&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B24&amp;"""",IF(Q$3=2,IF(B24=1,"true", "false"),B24))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC24" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD24" t="str">
-        <f>IF(ISBLANK(C24),"",AC24&amp;"}"&amp;IF(OR(AD25="]",AD25="",ISBLANK(AD25)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P25" t="str">
-        <f>IF(P$4=0,O25,O25&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A25&amp;"""",IF(P$3=2,IF(A25=1,"true", "false"),A25))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" ref="Q25:AC25" si="22">IF(Q$4=0,P25,P25&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B25&amp;"""",IF(Q$3=2,IF(B25=1,"true", "false"),B25))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q25:AC25" si="25">IF(Q$4=0,P25,P25&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B25&amp;"""",IF(Q$3=2,IF(B25=1,"true", "false"),B25))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC25" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD25" t="str">
-        <f>IF(ISBLANK(C25),"",AC25&amp;"}"&amp;IF(OR(AD26="]",AD26="",ISBLANK(AD26)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P26" t="str">
-        <f>IF(P$4=0,O26,O26&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A26&amp;"""",IF(P$3=2,IF(A26=1,"true", "false"),A26))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q26:AC26" si="23">IF(Q$4=0,P26,P26&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B26&amp;"""",IF(Q$3=2,IF(B26=1,"true", "false"),B26))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q26:AC26" si="26">IF(Q$4=0,P26,P26&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B26&amp;"""",IF(Q$3=2,IF(B26=1,"true", "false"),B26))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD26" t="str">
-        <f>IF(ISBLANK(C26),"",AC26&amp;"}"&amp;IF(OR(AD27="]",AD27="",ISBLANK(AD27)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P27" t="str">
-        <f>IF(P$4=0,O27,O27&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A27&amp;"""",IF(P$3=2,IF(A27=1,"true", "false"),A27))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ref="Q27:AC27" si="24">IF(Q$4=0,P27,P27&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B27&amp;"""",IF(Q$3=2,IF(B27=1,"true", "false"),B27))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q27:AC27" si="27">IF(Q$4=0,P27,P27&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B27&amp;"""",IF(Q$3=2,IF(B27=1,"true", "false"),B27))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC27" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD27" t="str">
-        <f>IF(ISBLANK(C27),"",AC27&amp;"}"&amp;IF(OR(AD28="]",AD28="",ISBLANK(AD28)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P28" t="str">
-        <f>IF(P$4=0,O28,O28&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A28&amp;"""",IF(P$3=2,IF(A28=1,"true", "false"),A28))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ref="Q28:AC28" si="25">IF(Q$4=0,P28,P28&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B28&amp;"""",IF(Q$3=2,IF(B28=1,"true", "false"),B28))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q28:AC28" si="28">IF(Q$4=0,P28,P28&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B28&amp;"""",IF(Q$3=2,IF(B28=1,"true", "false"),B28))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC28" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD28" t="str">
-        <f>IF(ISBLANK(C28),"",AC28&amp;"}"&amp;IF(OR(AD29="]",AD29="",ISBLANK(AD29)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P29" t="str">
-        <f>IF(P$4=0,O29,O29&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A29&amp;"""",IF(P$3=2,IF(A29=1,"true", "false"),A29))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q29:AC29" si="26">IF(Q$4=0,P29,P29&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B29&amp;"""",IF(Q$3=2,IF(B29=1,"true", "false"),B29))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q29:AC29" si="29">IF(Q$4=0,P29,P29&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B29&amp;"""",IF(Q$3=2,IF(B29=1,"true", "false"),B29))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC29" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD29" t="str">
-        <f>IF(ISBLANK(C29),"",AC29&amp;"}"&amp;IF(OR(AD30="]",AD30="",ISBLANK(AD30)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P30" t="str">
-        <f>IF(P$4=0,O30,O30&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A30&amp;"""",IF(P$3=2,IF(A30=1,"true", "false"),A30))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:AC30" si="27">IF(Q$4=0,P30,P30&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B30&amp;"""",IF(Q$3=2,IF(B30=1,"true", "false"),B30))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q30:AC30" si="30">IF(Q$4=0,P30,P30&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B30&amp;"""",IF(Q$3=2,IF(B30=1,"true", "false"),B30))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD30" t="str">
-        <f>IF(ISBLANK(C30),"",AC30&amp;"}"&amp;IF(OR(AD31="]",AD31="",ISBLANK(AD31)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P31" t="str">
-        <f>IF(P$4=0,O31,O31&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A31&amp;"""",IF(P$3=2,IF(A31=1,"true", "false"),A31))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" ref="Q31:AC31" si="28">IF(Q$4=0,P31,P31&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B31&amp;"""",IF(Q$3=2,IF(B31=1,"true", "false"),B31))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q31:AC31" si="31">IF(Q$4=0,P31,P31&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B31&amp;"""",IF(Q$3=2,IF(B31=1,"true", "false"),B31))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC31" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD31" t="str">
-        <f>IF(ISBLANK(C31),"",AC31&amp;"}"&amp;IF(OR(AD32="]",AD32="",ISBLANK(AD32)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P32" t="str">
-        <f>IF(P$4=0,O32,O32&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A32&amp;"""",IF(P$3=2,IF(A32=1,"true", "false"),A32))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ref="Q32:AC32" si="29">IF(Q$4=0,P32,P32&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B32&amp;"""",IF(Q$3=2,IF(B32=1,"true", "false"),B32))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q32:AC32" si="32">IF(Q$4=0,P32,P32&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B32&amp;"""",IF(Q$3=2,IF(B32=1,"true", "false"),B32))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD32" t="str">
-        <f>IF(ISBLANK(C32),"",AC32&amp;"}"&amp;IF(OR(AD33="]",AD33="",ISBLANK(AD33)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P33" t="str">
-        <f>IF(P$4=0,O33,O33&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A33&amp;"""",IF(P$3=2,IF(A33=1,"true", "false"),A33))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ref="Q33:AC33" si="30">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B33&amp;"""",IF(Q$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q33:AC33" si="33">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B33&amp;"""",IF(Q$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC33" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD33" t="str">
-        <f>IF(ISBLANK(C33),"",AC33&amp;"}"&amp;IF(OR(AD34="]",AD34="",ISBLANK(AD34)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P34" t="str">
-        <f>IF(P$4=0,O34,O34&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A34&amp;"""",IF(P$3=2,IF(A34=1,"true", "false"),A34))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ref="Q34:AC34" si="31">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B34&amp;"""",IF(Q$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q34:AC34" si="34">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B34&amp;"""",IF(Q$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC34" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD34" t="str">
-        <f>IF(ISBLANK(C34),"",AC34&amp;"}"&amp;IF(OR(AD35="]",AD35="",ISBLANK(AD35)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P35" t="str">
-        <f>IF(P$4=0,O35,O35&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A35&amp;"""",IF(P$3=2,IF(A35=1,"true", "false"),A35))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" ref="Q35:AC35" si="32">IF(Q$4=0,P35,P35&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B35&amp;"""",IF(Q$3=2,IF(B35=1,"true", "false"),B35))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q35:AC35" si="35">IF(Q$4=0,P35,P35&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B35&amp;"""",IF(Q$3=2,IF(B35=1,"true", "false"),B35))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC35" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD35" t="str">
-        <f>IF(ISBLANK(C35),"",AC35&amp;"}"&amp;IF(OR(AD36="]",AD36="",ISBLANK(AD36)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P36" t="str">
-        <f>IF(P$4=0,O36,O36&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A36&amp;"""",IF(P$3=2,IF(A36=1,"true", "false"),A36))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" ref="Q36:AC36" si="33">IF(Q$4=0,P36,P36&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B36&amp;"""",IF(Q$3=2,IF(B36=1,"true", "false"),B36))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q36:AC36" si="36">IF(Q$4=0,P36,P36&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B36&amp;"""",IF(Q$3=2,IF(B36=1,"true", "false"),B36))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD36" t="str">
-        <f>IF(ISBLANK(C36),"",AC36&amp;"}"&amp;IF(OR(AD37="]",AD37="",ISBLANK(AD37)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P37" t="str">
-        <f>IF(P$4=0,O37,O37&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A37&amp;"""",IF(P$3=2,IF(A37=1,"true", "false"),A37))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" ref="Q37:AC37" si="34">IF(Q$4=0,P37,P37&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B37&amp;"""",IF(Q$3=2,IF(B37=1,"true", "false"),B37))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q37:AC37" si="37">IF(Q$4=0,P37,P37&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B37&amp;"""",IF(Q$3=2,IF(B37=1,"true", "false"),B37))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD37" t="str">
-        <f>IF(ISBLANK(C37),"",AC37&amp;"}"&amp;IF(OR(AD38="]",AD38="",ISBLANK(AD38)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P38" t="str">
-        <f>IF(P$4=0,O38,O38&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A38&amp;"""",IF(P$3=2,IF(A38=1,"true", "false"),A38))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" ref="Q38:AC38" si="35">IF(Q$4=0,P38,P38&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B38&amp;"""",IF(Q$3=2,IF(B38=1,"true", "false"),B38))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q38:AC38" si="38">IF(Q$4=0,P38,P38&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B38&amp;"""",IF(Q$3=2,IF(B38=1,"true", "false"),B38))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC38" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD38" t="str">
-        <f>IF(ISBLANK(C38),"",AC38&amp;"}"&amp;IF(OR(AD39="]",AD39="",ISBLANK(AD39)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P39" t="str">
-        <f>IF(P$4=0,O39,O39&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A39&amp;"""",IF(P$3=2,IF(A39=1,"true", "false"),A39))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" ref="Q39:AC39" si="36">IF(Q$4=0,P39,P39&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B39&amp;"""",IF(Q$3=2,IF(B39=1,"true", "false"),B39))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q39:AC39" si="39">IF(Q$4=0,P39,P39&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B39&amp;"""",IF(Q$3=2,IF(B39=1,"true", "false"),B39))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD39" t="str">
-        <f>IF(ISBLANK(C39),"",AC39&amp;"}"&amp;IF(OR(AD40="]",AD40="",ISBLANK(AD40)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P40" t="str">
-        <f>IF(P$4=0,O40,O40&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A40&amp;"""",IF(P$3=2,IF(A40=1,"true", "false"),A40))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" ref="Q40:AC40" si="37">IF(Q$4=0,P40,P40&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B40&amp;"""",IF(Q$3=2,IF(B40=1,"true", "false"),B40))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q40:AC40" si="40">IF(Q$4=0,P40,P40&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B40&amp;"""",IF(Q$3=2,IF(B40=1,"true", "false"),B40))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC40" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD40" t="str">
-        <f>IF(ISBLANK(C40),"",AC40&amp;"}"&amp;IF(OR(AD41="]",AD41="",ISBLANK(AD41)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P41" t="str">
-        <f>IF(P$4=0,O41,O41&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A41&amp;"""",IF(P$3=2,IF(A41=1,"true", "false"),A41))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" ref="Q41:AC41" si="38">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B41&amp;"""",IF(Q$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q41:AC41" si="41">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B41&amp;"""",IF(Q$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC41" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD41" t="str">
-        <f>IF(ISBLANK(C41),"",AC41&amp;"}"&amp;IF(OR(AD42="]",AD42="",ISBLANK(AD42)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P42" t="str">
-        <f>IF(P$4=0,O42,O42&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A42&amp;"""",IF(P$3=2,IF(A42=1,"true", "false"),A42))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" ref="Q42:AC42" si="39">IF(Q$4=0,P42,P42&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B42&amp;"""",IF(Q$3=2,IF(B42=1,"true", "false"),B42))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q42:AC42" si="42">IF(Q$4=0,P42,P42&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B42&amp;"""",IF(Q$3=2,IF(B42=1,"true", "false"),B42))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC42" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD42" t="str">
-        <f>IF(ISBLANK(C42),"",AC42&amp;"}"&amp;IF(OR(AD43="]",AD43="",ISBLANK(AD43)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P43" t="str">
-        <f>IF(P$4=0,O43,O43&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A43&amp;"""",IF(P$3=2,IF(A43=1,"true", "false"),A43))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" ref="Q43:AC43" si="40">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B43&amp;"""",IF(Q$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q43:AC43" si="43">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B43&amp;"""",IF(Q$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC43" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD43" t="str">
-        <f>IF(ISBLANK(C43),"",AC43&amp;"}"&amp;IF(OR(AD44="]",AD44="",ISBLANK(AD44)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P44" t="str">
-        <f>IF(P$4=0,O44,O44&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A44&amp;"""",IF(P$3=2,IF(A44=1,"true", "false"),A44))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" ref="Q44:AC44" si="41">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B44&amp;"""",IF(Q$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q44:AC44" si="44">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B44&amp;"""",IF(Q$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC44" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD44" t="str">
-        <f>IF(ISBLANK(C44),"",AC44&amp;"}"&amp;IF(OR(AD45="]",AD45="",ISBLANK(AD45)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P45" t="str">
-        <f>IF(P$4=0,O45,O45&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A45&amp;"""",IF(P$3=2,IF(A45=1,"true", "false"),A45))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" ref="Q45:AC45" si="42">IF(Q$4=0,P45,P45&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B45&amp;"""",IF(Q$3=2,IF(B45=1,"true", "false"),B45))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q45:AC45" si="45">IF(Q$4=0,P45,P45&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B45&amp;"""",IF(Q$3=2,IF(B45=1,"true", "false"),B45))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC45" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD45" t="str">
-        <f>IF(ISBLANK(C45),"",AC45&amp;"}"&amp;IF(OR(AD46="]",AD46="",ISBLANK(AD46)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="15:30" x14ac:dyDescent="0.2">
       <c r="O46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P46" t="str">
-        <f>IF(P$4=0,O46,O46&amp;IF(ISBLANK(O$3),"",",")&amp;""""&amp;A$4&amp;""":"&amp;IF(P$3=1,""""&amp;A46&amp;"""",IF(P$3=2,IF(A46=1,"true", "false"),A46))&amp;IF(ISBLANK(Q$3),"},",""))</f>
+        <f t="shared" si="1"/>
         <v>{"user":""</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" ref="Q46:AC46" si="43">IF(Q$4=0,P46,P46&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B46&amp;"""",IF(Q$3=2,IF(B46=1,"true", "false"),B46))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q46:AC46" si="46">IF(Q$4=0,P46,P46&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B46&amp;"""",IF(Q$3=2,IF(B46=1,"true", "false"),B46))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC46" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD46" t="str">
-        <f>IF(ISBLANK(C46),"",AC46&amp;"}"&amp;IF(OR(AD47="]",AD47="",ISBLANK(AD47)),"",","))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
update manager to emploji
</commit_message>
<xml_diff>
--- a/import/datastore/users.xlsx
+++ b/import/datastore/users.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="104">
   <si>
     <t>ski</t>
   </si>
@@ -325,6 +325,24 @@
   </si>
   <si>
     <t>Bot</t>
+  </si>
+  <si>
+    <t>emploji</t>
+  </si>
+  <si>
+    <t>U5BA7L6JE:T5C4WRWET</t>
+  </si>
+  <si>
+    <t>Emploji</t>
+  </si>
+  <si>
+    <t>2017-06-08</t>
+  </si>
+  <si>
+    <t>Slack user</t>
+  </si>
+  <si>
+    <t>Slack</t>
   </si>
 </sst>
 </file>
@@ -504,7 +522,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,7 +534,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -659,7 +676,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -714,7 +731,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -769,7 +786,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -826,7 +843,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -883,7 +900,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -940,7 +957,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -995,7 +1012,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1052,7 +1069,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1107,7 +1124,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1164,7 +1181,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1221,7 +1238,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1278,7 +1295,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1333,7 +1350,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1390,7 +1407,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1445,7 +1462,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1500,7 +1517,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1555,7 +1572,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1612,7 +1629,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1667,7 +1684,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1722,7 +1739,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1779,7 +1796,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1834,7 +1851,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1889,7 +1906,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1946,7 +1963,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2003,7 +2020,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2060,7 +2077,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2115,7 +2132,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2172,7 +2189,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2227,7 +2244,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2282,7 +2299,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2337,7 +2354,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2394,7 +2411,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2449,7 +2466,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2504,7 +2521,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2561,7 +2578,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2616,7 +2633,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2671,7 +2688,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2728,7 +2745,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2785,7 +2802,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2842,7 +2859,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3180,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4:AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3435,7 +3452,7 @@
         <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O5" t="str">
         <f>"{"</f>
@@ -3487,19 +3504,19 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
+        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"emploji"</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
+        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"emploji"</v>
       </c>
       <c r="AC5" t="str">
         <f t="shared" si="2"/>
-        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"</v>
+        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"emploji"</v>
       </c>
       <c r="AD5" t="str">
-        <f t="shared" ref="AD5:AD12" si="3">IF(ISBLANK(C5),"",AC5&amp;"}"&amp;IF(OR(AD6="]",AD6="",ISBLANK(AD6)),"",","))</f>
-        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"david"},</v>
+        <f t="shared" ref="AD5:AD46" si="3">IF(ISBLANK(C5),"",AC5&amp;"}"&amp;IF(OR(AD6="]",AD6="",ISBLANK(AD6)),"",","))</f>
+        <v>{"user":"meyerchri","slack_id":"U5L3D6A6L:T5C4WRWET","name":"Meyer","firstname":"Christina","dateOfBirth":"1969-04-13","minExpenses":"0","position":"Innovation","Anstellung":"60","sex":"f","kostenstelle":"10133","kostenstelle_bezeichnung":"Innovation","manager":"emploji"},</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -3537,7 +3554,7 @@
         <v>79</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" ref="O6:O46" si="4">"{"</f>
@@ -3589,19 +3606,19 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"emploji"</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"emploji"</v>
       </c>
       <c r="AC6" t="str">
         <f t="shared" si="5"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"</v>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"emploji"</v>
       </c>
       <c r="AD6" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"lorenz-haenggi"},</v>
+        <v>{"user":"david","slack_id":"U5EPZJE92:T5C4WRWET","name":"Ulrich","firstname":"David","dateOfBirth":"1970-04-01","minExpenses":"50","position":"Architecture","Anstellung":"90","sex":"m","kostenstelle":"18327","kostenstelle_bezeichnung":"IT Strategy a.Archit","manager":"emploji"},</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -3639,7 +3656,7 @@
         <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="4"/>
@@ -3691,19 +3708,19 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
+        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"emploji"</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
+        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"emploji"</v>
       </c>
       <c r="AC7" t="str">
         <f t="shared" si="6"/>
-        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"</v>
+        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"emploji"</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"david"},</v>
+        <v>{"user":"remostrupler","slack_id":"U5EM8E86P:T5C4WRWET","name":"Struppler","firstname":"Remo","dateOfBirth":"1950-01-01","minExpenses":"0","position":"IT-Risk","Anstellung":"100","sex":"m","kostenstelle":"18328","kostenstelle_bezeichnung":"IT Fin. &amp; Risk. Man.","manager":"emploji"},</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -3741,7 +3758,7 @@
         <v>81</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="4"/>
@@ -3793,19 +3810,19 @@
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
+        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"emploji"</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
+        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"emploji"</v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="7"/>
-        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"</v>
+        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"emploji"</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"david"},</v>
+        <v>{"user":"susanne_s","slack_id":"U5LL0BN4U:T5C4WRWET","name":"Sulzer","firstname":"Susanne","dateOfBirth":"1950-01-01","minExpenses":"0","position":"HR","Anstellung":"100","sex":"f","kostenstelle":"18201","kostenstelle_bezeichnung":"Employee Services","manager":"emploji"},</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -3843,7 +3860,7 @@
         <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="4"/>
@@ -3895,19 +3912,19 @@
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
+        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"emploji"</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
+        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"emploji"</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="8"/>
-        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"</v>
+        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"emploji"</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"david"},</v>
+        <v>{"user":"lorenz-haenggi","slack_id":"U5BBP86RJ:T5C4WRWET","name":"Hänggi","firstname":"Lorenz","dateOfBirth":"1969-04-13","minExpenses":"50","position":"Innovation","Anstellung":"100","sex":"m","kostenstelle":"18323","kostenstelle_bezeichnung":"Sales and Digital BA","manager":"emploji"},</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -3945,7 +3962,7 @@
         <v>83</v>
       </c>
       <c r="L10" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="4"/>
@@ -3997,19 +4014,19 @@
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
+        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"emploji"</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
+        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"emploji"</v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="9"/>
-        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"</v>
+        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"emploji"</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"david"},</v>
+        <v>{"user":"cogji","slack_id":"U5GEGT83C:T5C4WRWET","name":"Giorgi","firstname":"Corinne","dateOfBirth":"1960-01-01","minExpenses":"0","position":"HR","Anstellung":"80","sex":"f","kostenstelle":"18222","kostenstelle_bezeichnung":"People Development","manager":"emploji"},</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -4047,7 +4064,7 @@
         <v>84</v>
       </c>
       <c r="L11" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="4"/>
@@ -4099,19 +4116,19 @@
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
+        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"emploji"</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
+        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"emploji"</v>
       </c>
       <c r="AC11" t="str">
         <f t="shared" si="10"/>
-        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"</v>
+        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"emploji"</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"david"},</v>
+        <v>{"user":"brm","slack_id":"U5Q62U63V:T5C4WRWET","name":"Breitenmoser","firstname":"Bernhard","dateOfBirth":"1960-01-01","minExpenses":"0","position":"SAP Specialist","Anstellung":"100","sex":"m","kostenstelle":"SCHB1001","kostenstelle_bezeichnung":"SAP Common Services","manager":"emploji"},</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -4127,8 +4144,8 @@
       <c r="D12" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="11">
-        <v>42894</v>
+      <c r="E12" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -4149,7 +4166,7 @@
         <v>97</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="4"/>
@@ -4173,113 +4190,149 @@
       </c>
       <c r="T12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08"</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0"</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot"</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100"</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222"</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot"</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"emploji"</v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"emploji"</v>
       </c>
       <c r="AC12" t="str">
         <f t="shared" si="11"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"emploji"</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="3"/>
-        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"42894","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"remostrupler"}</v>
+        <v>{"user":"User","slack_id":"default-user","name":"Emulator","firstname":"Botly","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Bot","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Bot","manager":"emploji"},</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13">
+        <v>18222</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" t="s">
+        <v>98</v>
+      </c>
       <c r="O13" t="str">
         <f t="shared" si="4"/>
         <v>{</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="1"/>
-        <v>{"user":""</v>
+        <v>{"user":"emploji"</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" ref="Q13:AC13" si="12">IF(Q$4=0,P13,P13&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B13&amp;"""",IF(Q$3=2,IF(B13=1,"true", "false"),B13))&amp;IF(ISBLANK(R$3),"},",""))</f>
-        <v>{"user":"","slack_id":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET"</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji"</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot"</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08"</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0"</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user"</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100"</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m"</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222"</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Slack"</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Slack","manager":"emploji"</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Slack","manager":"emploji"</v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="12"/>
-        <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Slack","manager":"emploji"</v>
       </c>
       <c r="AD13" t="str">
-        <f>IF(ISBLANK(C13),"",AC13&amp;"}"&amp;IF(OR(#REF!="]",#REF!="",ISBLANK(#REF!)),"",","))</f>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>{"user":"emploji","slack_id":"U5BA7L6JE:T5C4WRWET","name":"Emploji","firstname":"Bot","dateOfBirth":"2017-06-08","minExpenses":"0","position":"Slack user","Anstellung":"100","sex":"m","kostenstelle":"18222","kostenstelle_bezeichnung":"Slack","manager":"emploji"}</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -4344,7 +4397,7 @@
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD14" t="str">
-        <f t="shared" ref="AD14:AD46" si="14">IF(ISBLANK(C14),"",AC14&amp;"}"&amp;IF(OR(AD15="]",AD15="",ISBLANK(AD15)),"",","))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4358,59 +4411,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" ref="Q15:AC15" si="15">IF(Q$4=0,P15,P15&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B15&amp;"""",IF(Q$3=2,IF(B15=1,"true", "false"),B15))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q15:AC15" si="14">IF(Q$4=0,P15,P15&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B15&amp;"""",IF(Q$3=2,IF(B15=1,"true", "false"),B15))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4424,59 +4477,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" ref="Q16:AC16" si="16">IF(Q$4=0,P16,P16&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B16&amp;"""",IF(Q$3=2,IF(B16=1,"true", "false"),B16))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q16:AC16" si="15">IF(Q$4=0,P16,P16&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B16&amp;"""",IF(Q$3=2,IF(B16=1,"true", "false"),B16))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD16" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4490,59 +4543,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" ref="Q17:AC17" si="17">IF(Q$4=0,P17,P17&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B17&amp;"""",IF(Q$3=2,IF(B17=1,"true", "false"),B17))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q17:AC17" si="16">IF(Q$4=0,P17,P17&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B17&amp;"""",IF(Q$3=2,IF(B17=1,"true", "false"),B17))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC17" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4556,59 +4609,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" ref="Q18:AC18" si="18">IF(Q$4=0,P18,P18&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B18&amp;"""",IF(Q$3=2,IF(B18=1,"true", "false"),B18))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q18:AC18" si="17">IF(Q$4=0,P18,P18&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B18&amp;"""",IF(Q$3=2,IF(B18=1,"true", "false"),B18))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4622,59 +4675,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" ref="Q19:AC19" si="19">IF(Q$4=0,P19,P19&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B19&amp;"""",IF(Q$3=2,IF(B19=1,"true", "false"),B19))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q19:AC19" si="18">IF(Q$4=0,P19,P19&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B19&amp;"""",IF(Q$3=2,IF(B19=1,"true", "false"),B19))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC19" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD19" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4688,59 +4741,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ref="Q20:AC20" si="20">IF(Q$4=0,P20,P20&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B20&amp;"""",IF(Q$3=2,IF(B20=1,"true", "false"),B20))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q20:AC20" si="19">IF(Q$4=0,P20,P20&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B20&amp;"""",IF(Q$3=2,IF(B20=1,"true", "false"),B20))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC20" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD20" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4754,59 +4807,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" ref="Q21:AC21" si="21">IF(Q$4=0,P21,P21&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B21&amp;"""",IF(Q$3=2,IF(B21=1,"true", "false"),B21))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q21:AC21" si="20">IF(Q$4=0,P21,P21&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B21&amp;"""",IF(Q$3=2,IF(B21=1,"true", "false"),B21))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC21" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD21" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4820,59 +4873,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22:AC22" si="22">IF(Q$4=0,P22,P22&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B22&amp;"""",IF(Q$3=2,IF(B22=1,"true", "false"),B22))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q22:AC22" si="21">IF(Q$4=0,P22,P22&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B22&amp;"""",IF(Q$3=2,IF(B22=1,"true", "false"),B22))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC22" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4886,59 +4939,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" ref="Q23:AC23" si="23">IF(Q$4=0,P23,P23&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B23&amp;"""",IF(Q$3=2,IF(B23=1,"true", "false"),B23))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q23:AC23" si="22">IF(Q$4=0,P23,P23&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B23&amp;"""",IF(Q$3=2,IF(B23=1,"true", "false"),B23))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC23" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD23" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4952,59 +5005,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" ref="Q24:AC24" si="24">IF(Q$4=0,P24,P24&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B24&amp;"""",IF(Q$3=2,IF(B24=1,"true", "false"),B24))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q24:AC24" si="23">IF(Q$4=0,P24,P24&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B24&amp;"""",IF(Q$3=2,IF(B24=1,"true", "false"),B24))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD24" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5018,59 +5071,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" ref="Q25:AC25" si="25">IF(Q$4=0,P25,P25&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B25&amp;"""",IF(Q$3=2,IF(B25=1,"true", "false"),B25))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q25:AC25" si="24">IF(Q$4=0,P25,P25&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B25&amp;"""",IF(Q$3=2,IF(B25=1,"true", "false"),B25))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD25" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5084,59 +5137,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q26:AC26" si="26">IF(Q$4=0,P26,P26&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B26&amp;"""",IF(Q$3=2,IF(B26=1,"true", "false"),B26))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q26:AC26" si="25">IF(Q$4=0,P26,P26&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B26&amp;"""",IF(Q$3=2,IF(B26=1,"true", "false"),B26))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5150,59 +5203,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ref="Q27:AC27" si="27">IF(Q$4=0,P27,P27&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B27&amp;"""",IF(Q$3=2,IF(B27=1,"true", "false"),B27))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q27:AC27" si="26">IF(Q$4=0,P27,P27&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B27&amp;"""",IF(Q$3=2,IF(B27=1,"true", "false"),B27))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5216,59 +5269,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ref="Q28:AC28" si="28">IF(Q$4=0,P28,P28&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B28&amp;"""",IF(Q$3=2,IF(B28=1,"true", "false"),B28))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q28:AC28" si="27">IF(Q$4=0,P28,P28&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B28&amp;"""",IF(Q$3=2,IF(B28=1,"true", "false"),B28))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC28" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5282,59 +5335,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q29:AC29" si="29">IF(Q$4=0,P29,P29&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B29&amp;"""",IF(Q$3=2,IF(B29=1,"true", "false"),B29))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q29:AC29" si="28">IF(Q$4=0,P29,P29&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B29&amp;"""",IF(Q$3=2,IF(B29=1,"true", "false"),B29))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC29" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD29" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5348,59 +5401,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:AC30" si="30">IF(Q$4=0,P30,P30&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B30&amp;"""",IF(Q$3=2,IF(B30=1,"true", "false"),B30))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q30:AC30" si="29">IF(Q$4=0,P30,P30&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B30&amp;"""",IF(Q$3=2,IF(B30=1,"true", "false"),B30))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC30" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD30" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5414,59 +5467,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" ref="Q31:AC31" si="31">IF(Q$4=0,P31,P31&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B31&amp;"""",IF(Q$3=2,IF(B31=1,"true", "false"),B31))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q31:AC31" si="30">IF(Q$4=0,P31,P31&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B31&amp;"""",IF(Q$3=2,IF(B31=1,"true", "false"),B31))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC31" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD31" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5480,59 +5533,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ref="Q32:AC32" si="32">IF(Q$4=0,P32,P32&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B32&amp;"""",IF(Q$3=2,IF(B32=1,"true", "false"),B32))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q32:AC32" si="31">IF(Q$4=0,P32,P32&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B32&amp;"""",IF(Q$3=2,IF(B32=1,"true", "false"),B32))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC32" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5546,59 +5599,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ref="Q33:AC33" si="33">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B33&amp;"""",IF(Q$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q33:AC33" si="32">IF(Q$4=0,P33,P33&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B33&amp;"""",IF(Q$3=2,IF(B33=1,"true", "false"),B33))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC33" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5612,59 +5665,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ref="Q34:AC34" si="34">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B34&amp;"""",IF(Q$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q34:AC34" si="33">IF(Q$4=0,P34,P34&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B34&amp;"""",IF(Q$3=2,IF(B34=1,"true", "false"),B34))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC34" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD34" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5678,59 +5731,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" ref="Q35:AC35" si="35">IF(Q$4=0,P35,P35&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B35&amp;"""",IF(Q$3=2,IF(B35=1,"true", "false"),B35))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q35:AC35" si="34">IF(Q$4=0,P35,P35&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B35&amp;"""",IF(Q$3=2,IF(B35=1,"true", "false"),B35))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC35" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5744,59 +5797,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" ref="Q36:AC36" si="36">IF(Q$4=0,P36,P36&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B36&amp;"""",IF(Q$3=2,IF(B36=1,"true", "false"),B36))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q36:AC36" si="35">IF(Q$4=0,P36,P36&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B36&amp;"""",IF(Q$3=2,IF(B36=1,"true", "false"),B36))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD36" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5810,59 +5863,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" ref="Q37:AC37" si="37">IF(Q$4=0,P37,P37&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B37&amp;"""",IF(Q$3=2,IF(B37=1,"true", "false"),B37))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q37:AC37" si="36">IF(Q$4=0,P37,P37&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B37&amp;"""",IF(Q$3=2,IF(B37=1,"true", "false"),B37))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC37" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5876,59 +5929,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" ref="Q38:AC38" si="38">IF(Q$4=0,P38,P38&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B38&amp;"""",IF(Q$3=2,IF(B38=1,"true", "false"),B38))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q38:AC38" si="37">IF(Q$4=0,P38,P38&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B38&amp;"""",IF(Q$3=2,IF(B38=1,"true", "false"),B38))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC38" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD38" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5942,59 +5995,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" ref="Q39:AC39" si="39">IF(Q$4=0,P39,P39&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B39&amp;"""",IF(Q$3=2,IF(B39=1,"true", "false"),B39))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q39:AC39" si="38">IF(Q$4=0,P39,P39&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B39&amp;"""",IF(Q$3=2,IF(B39=1,"true", "false"),B39))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC39" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD39" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6008,59 +6061,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" ref="Q40:AC40" si="40">IF(Q$4=0,P40,P40&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B40&amp;"""",IF(Q$3=2,IF(B40=1,"true", "false"),B40))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q40:AC40" si="39">IF(Q$4=0,P40,P40&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B40&amp;"""",IF(Q$3=2,IF(B40=1,"true", "false"),B40))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC40" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6074,59 +6127,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" ref="Q41:AC41" si="41">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B41&amp;"""",IF(Q$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q41:AC41" si="40">IF(Q$4=0,P41,P41&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B41&amp;"""",IF(Q$3=2,IF(B41=1,"true", "false"),B41))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC41" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD41" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6140,59 +6193,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" ref="Q42:AC42" si="42">IF(Q$4=0,P42,P42&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B42&amp;"""",IF(Q$3=2,IF(B42=1,"true", "false"),B42))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q42:AC42" si="41">IF(Q$4=0,P42,P42&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B42&amp;"""",IF(Q$3=2,IF(B42=1,"true", "false"),B42))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC42" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD42" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6206,59 +6259,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" ref="Q43:AC43" si="43">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B43&amp;"""",IF(Q$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q43:AC43" si="42">IF(Q$4=0,P43,P43&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B43&amp;"""",IF(Q$3=2,IF(B43=1,"true", "false"),B43))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC43" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD43" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6272,59 +6325,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" ref="Q44:AC44" si="44">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B44&amp;"""",IF(Q$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q44:AC44" si="43">IF(Q$4=0,P44,P44&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B44&amp;"""",IF(Q$3=2,IF(B44=1,"true", "false"),B44))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC44" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6338,59 +6391,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" ref="Q45:AC45" si="45">IF(Q$4=0,P45,P45&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B45&amp;"""",IF(Q$3=2,IF(B45=1,"true", "false"),B45))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q45:AC45" si="44">IF(Q$4=0,P45,P45&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B45&amp;"""",IF(Q$3=2,IF(B45=1,"true", "false"),B45))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC45" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD45" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6404,59 +6457,59 @@
         <v>{"user":""</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" ref="Q46:AC46" si="46">IF(Q$4=0,P46,P46&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B46&amp;"""",IF(Q$3=2,IF(B46=1,"true", "false"),B46))&amp;IF(ISBLANK(R$3),"},",""))</f>
+        <f t="shared" ref="Q46:AC46" si="45">IF(Q$4=0,P46,P46&amp;IF(ISBLANK(P$3),"",",")&amp;""""&amp;B$4&amp;""":"&amp;IF(Q$3=1,""""&amp;B46&amp;"""",IF(Q$3=2,IF(B46=1,"true", "false"),B46))&amp;IF(ISBLANK(R$3),"},",""))</f>
         <v>{"user":"","slack_id":""</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":""</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":""</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":""</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":""</v>
       </c>
       <c r="V46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":""</v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":""</v>
       </c>
       <c r="X46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":""</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":""</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":""</v>
       </c>
       <c r="AA46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AB46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AC46" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>{"user":"","slack_id":"","name":"","firstname":"","dateOfBirth":"","minExpenses":"","position":"","Anstellung":"","sex":"","kostenstelle":"","kostenstelle_bezeichnung":"","manager":""</v>
       </c>
       <c r="AD46" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>

</xml_diff>